<commit_message>
Version con DataService y mejoras
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ClonedRepos\Frameworks\ExtendedREFramework_ColectorExcel\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ClonedRepos\Frameworks\ExtendedREFramework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="3"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="139">
   <si>
     <t>Name</t>
   </si>
@@ -304,9 +304,6 @@
     <t>MailProcessNickName</t>
   </si>
   <si>
-    <t>Dora</t>
-  </si>
-  <si>
     <t>PRN</t>
   </si>
   <si>
@@ -340,6 +337,15 @@
     <t>ProcessModule</t>
   </si>
   <si>
+    <t>Colector/Consumidor</t>
+  </si>
+  <si>
+    <t>MailContactLanguage</t>
+  </si>
+  <si>
+    <t>es-ES</t>
+  </si>
+  <si>
     <t>MailTO_All</t>
   </si>
   <si>
@@ -358,31 +364,19 @@
     <t>MailBCC_Exceptions</t>
   </si>
   <si>
-    <t>Colector/Consumidor</t>
-  </si>
-  <si>
-    <t>MailContactLanguage</t>
-  </si>
-  <si>
-    <t>es-ES</t>
+    <t>CAMBIAR</t>
   </si>
   <si>
     <t>SendMail</t>
   </si>
   <si>
-    <t>MailFailColector</t>
-  </si>
-  <si>
-    <t>Reporte de ejecución colector - Hay KOs!</t>
-  </si>
-  <si>
-    <t>MailOKColector</t>
-  </si>
-  <si>
-    <t>Reporte de ejecución colector - Todo OK</t>
-  </si>
-  <si>
     <t>QueueNameNextStep</t>
+  </si>
+  <si>
+    <t>ItemTableNextStep</t>
+  </si>
+  <si>
+    <t>Name of the "main" Database table for the next step</t>
   </si>
   <si>
     <r>
@@ -408,34 +402,67 @@
     </r>
   </si>
   <si>
-    <t>ItemTableNextStep</t>
-  </si>
-  <si>
-    <t>Name of the "main" Database table for the next step</t>
-  </si>
-  <si>
-    <t>CAMBIAR</t>
-  </si>
-  <si>
-    <t>Constantes Carpetas</t>
-  </si>
-  <si>
-    <t>No Cambiar</t>
+    <t>NO CAMBIAR</t>
+  </si>
+  <si>
+    <t>ConstantesCarpetas</t>
+  </si>
+  <si>
+    <t>RPA_DBConnectionString</t>
+  </si>
+  <si>
+    <t>RPA_SharedFolder_Base</t>
+  </si>
+  <si>
+    <t>RPA_SMTPHost</t>
+  </si>
+  <si>
+    <t>RPA_SMTPPort</t>
   </si>
   <si>
     <t>NoReply</t>
   </si>
   <si>
-    <t>RPA_SharedFolder_Base</t>
-  </si>
-  <si>
-    <t>RPA_SMTPHost</t>
-  </si>
-  <si>
-    <t>RPA_SMTPPort</t>
-  </si>
-  <si>
-    <t>RPA_DBConnectionString</t>
+    <t>UseDB</t>
+  </si>
+  <si>
+    <t>Use auxiliary database for error codes and item data</t>
+  </si>
+  <si>
+    <t>UseDataServiceErrors</t>
+  </si>
+  <si>
+    <t>UseDataServiceItem</t>
+  </si>
+  <si>
+    <t>Use Data service for item data</t>
+  </si>
+  <si>
+    <t>Use Data service for error codes</t>
+  </si>
+  <si>
+    <t>ExceptionLanguage</t>
+  </si>
+  <si>
+    <t>EnforceSecondDataSource</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If set to true, framework will attempt to get data from relevant data source (DB/Data Service). If data doesn't exist, an exception will be htrown . If false, it will not try to retrieve data from data source </t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Windows(\)</t>
+  </si>
+  <si>
+    <t>Unix(/)</t>
+  </si>
+  <si>
+    <t>Add failed items to next queue already as failed</t>
+  </si>
+  <si>
+    <t>AddFailedItem</t>
   </si>
 </sst>
 </file>
@@ -834,18 +861,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z1012"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -895,152 +922,222 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="45">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="43.5">
+      <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="4" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="30">
-      <c r="A6" t="s">
+    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="29">
+      <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>52</v>
-      </c>
+    <row r="8" spans="1:26" ht="14.5">
+      <c r="B8" s="2"/>
+      <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>120</v>
+        <v>125</v>
+      </c>
+      <c r="B9" t="b">
+        <v>0</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>102</v>
+      <c r="A12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B12" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>102</v>
+      <c r="A13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B13" t="b">
+        <v>1</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>106</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>102</v>
+        <v>132</v>
+      </c>
+      <c r="B14" t="b">
+        <v>1</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B21" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>108</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" t="s">
+        <v>109</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
+        <v>111</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="B26" s="8"/>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A27" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A17" t="s">
-        <v>109</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="14.25" customHeight="1">
-      <c r="B18" s="8"/>
-    </row>
-    <row r="19" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A19" t="s">
+      <c r="B27" t="s">
         <v>103</v>
       </c>
-      <c r="B19" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A21" t="s">
-        <v>111</v>
-      </c>
-      <c r="B21" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A22" t="s">
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A29" t="s">
+        <v>104</v>
+      </c>
+      <c r="B29" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A30" t="s">
         <v>113</v>
       </c>
-      <c r="B22" t="b">
+      <c r="B30" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -2007,6 +2104,20 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
+    <row r="1000" ht="14.25" customHeight="1"/>
+    <row r="1001" ht="14.25" customHeight="1"/>
+    <row r="1002" ht="14.25" customHeight="1"/>
+    <row r="1003" ht="14.25" customHeight="1"/>
+    <row r="1004" ht="14.25" customHeight="1"/>
+    <row r="1005" ht="14.25" customHeight="1"/>
+    <row r="1006" ht="14.25" customHeight="1"/>
+    <row r="1007" ht="14.25" customHeight="1"/>
+    <row r="1008" ht="14.25" customHeight="1"/>
+    <row r="1009" ht="14.25" customHeight="1"/>
+    <row r="1010" ht="14.25" customHeight="1"/>
+    <row r="1011" ht="14.25" customHeight="1"/>
+    <row r="1012" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2016,18 +2127,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z953"/>
+  <dimension ref="A1:Z951"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2064,18 +2175,18 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -2189,7 +2300,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -2201,12 +2312,12 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A19" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>124</v>
+    <row r="19" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A19" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
@@ -2332,10 +2443,10 @@
     </row>
     <row r="35" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
       <c r="A35" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>122</v>
+        <v>97</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1">
@@ -2343,7 +2454,7 @@
         <v>89</v>
       </c>
       <c r="B36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C36" t="s">
         <v>88</v>
@@ -2354,7 +2465,7 @@
         <v>90</v>
       </c>
       <c r="B37" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C37" t="s">
         <v>88</v>
@@ -2365,7 +2476,7 @@
         <v>91</v>
       </c>
       <c r="B38" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="C38" t="s">
         <v>88</v>
@@ -2373,47 +2484,33 @@
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" t="s">
+        <v>124</v>
+      </c>
+      <c r="C39" t="s">
         <v>94</v>
-      </c>
-      <c r="B39" t="s">
-        <v>125</v>
-      </c>
-      <c r="C39" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1">
       <c r="A40" t="s">
+        <v>95</v>
+      </c>
+      <c r="B40" t="s">
         <v>96</v>
-      </c>
-      <c r="B40" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="A41" t="s">
+        <v>98</v>
+      </c>
+      <c r="B41" t="s">
         <v>99</v>
       </c>
-      <c r="B41" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A42" t="s">
-        <v>114</v>
-      </c>
-      <c r="B42" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A43" t="s">
-        <v>116</v>
-      </c>
-      <c r="B43" t="s">
-        <v>117</v>
-      </c>
-    </row>
+    </row>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3322,8 +3419,6 @@
     <row r="949" ht="14.25" customHeight="1"/>
     <row r="950" ht="14.25" customHeight="1"/>
     <row r="951" ht="14.25" customHeight="1"/>
-    <row r="952" ht="14.25" customHeight="1"/>
-    <row r="953" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3339,12 +3434,12 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
+    <col min="2" max="2" width="30.1796875" customWidth="1"/>
+    <col min="3" max="3" width="60.26953125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3388,7 +3483,7 @@
         <v>84</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C2" t="s">
         <v>60</v>
@@ -3402,7 +3497,7 @@
         <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C3" t="s">
         <v>60</v>
@@ -3413,7 +3508,7 @@
         <v>54</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C4" t="s">
         <v>60</v>
@@ -4424,16 +4519,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
+    <col min="2" max="2" width="30.1796875" customWidth="1"/>
+    <col min="3" max="3" width="60.26953125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -4477,7 +4572,7 @@
         <v>45</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C2" t="s">
         <v>60</v>
@@ -5498,20 +5593,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:AA998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
+    <col min="2" max="3" width="60.26953125" customWidth="1"/>
+    <col min="4" max="4" width="15.90625" customWidth="1"/>
+    <col min="5" max="27" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14.25" customHeight="1">
+    <row r="1" spans="1:27" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5522,9 +5618,11 @@
         <v>44</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -5546,24 +5644,34 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
-    </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="AA1" s="1"/>
+    </row>
+    <row r="2" spans="1:27" ht="14.25" customHeight="1">
+      <c r="D2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="14.25" customHeight="1">
+      <c r="D3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:27" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:27" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:27" ht="14.25" customHeight="1">
       <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:27" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:27" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:27" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:27" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:27" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:27" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:27" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:27" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:27" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -6547,6 +6655,11 @@
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
+      <formula1>"Windows(\),Unix(/)"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added test cases, local errors
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ClonedRepos\Frameworks\ExtendedREFramework\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ClonedRepos\Frameworks\ExtendedREFramework_ColectorExcel\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="141">
   <si>
     <t>Name</t>
   </si>
@@ -463,6 +463,12 @@
   </si>
   <si>
     <t>AddFailedItem</t>
+  </si>
+  <si>
+    <t>ErrorCodePath</t>
+  </si>
+  <si>
+    <t>Data\ErrorCodes.xlsx</t>
   </si>
 </sst>
 </file>
@@ -863,16 +869,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -940,7 +946,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="43.5">
+    <row r="5" spans="1:26" ht="45">
       <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
@@ -950,7 +956,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="29">
+    <row r="7" spans="1:26" ht="30">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -961,7 +967,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.5">
+    <row r="8" spans="1:26">
       <c r="B8" s="2"/>
       <c r="C8" s="4"/>
     </row>
@@ -1137,7 +1143,14 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A32" t="s">
+        <v>139</v>
+      </c>
+      <c r="B32" t="s">
+        <v>140</v>
+      </c>
+    </row>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -2133,12 +2146,12 @@
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2175,7 +2188,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="29">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2186,7 +2199,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -2300,7 +2313,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="29">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -3434,12 +3447,12 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" customWidth="1"/>
-    <col min="2" max="2" width="30.1796875" customWidth="1"/>
-    <col min="3" max="3" width="60.26953125" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -4523,12 +4536,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" customWidth="1"/>
-    <col min="2" max="2" width="30.1796875" customWidth="1"/>
-    <col min="3" max="3" width="60.26953125" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -5599,12 +5612,12 @@
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" customWidth="1"/>
-    <col min="2" max="3" width="60.26953125" customWidth="1"/>
-    <col min="4" max="4" width="15.90625" customWidth="1"/>
-    <col min="5" max="27" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="27" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Added Colector Report Added Docs Addded Process.xaml
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="141">
   <si>
     <t>Name</t>
   </si>
@@ -88,15 +88,7 @@
     <t>logF_BusinessProcessName</t>
   </si>
   <si>
-    <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>OrchestratorQueueName</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -469,6 +461,12 @@
   </si>
   <si>
     <t>Data\ErrorCodes.xlsx</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueName</t>
+  </si>
+  <si>
+    <t>Orchestrator queue Name. This will be the Queue where items are loaded</t>
   </si>
 </sst>
 </file>
@@ -869,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -917,42 +915,44 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>21</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B3" s="2"/>
+        <v>112</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="C3" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B4" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="45">
       <c r="A5" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
@@ -961,10 +961,10 @@
         <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -973,73 +973,73 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B9" t="b">
         <v>0</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C15" s="4"/>
     </row>
@@ -1051,13 +1051,13 @@
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
@@ -1067,51 +1067,51 @@
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
@@ -1119,36 +1119,36 @@
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B32" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33" ht="14.25" customHeight="1"/>
@@ -2142,8 +2142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z951"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2196,18 +2196,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2231,7 +2231,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -2253,7 +2253,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -2264,7 +2264,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -2275,173 +2275,173 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B17" t="b">
         <v>1</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="19" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
       <c r="A19" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" t="s">
         <v>56</v>
       </c>
-      <c r="B20" t="s">
-        <v>58</v>
-      </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" t="s">
         <v>62</v>
-      </c>
-      <c r="B22" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" t="s">
         <v>63</v>
-      </c>
-      <c r="B23" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B27" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="C30" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
       <c r="A31" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="C31" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1">
@@ -2456,70 +2456,70 @@
     </row>
     <row r="35" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
       <c r="A35" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1">
       <c r="A36" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B36" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C36" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1">
       <c r="A37" t="s">
+        <v>88</v>
+      </c>
+      <c r="B37" t="s">
         <v>90</v>
       </c>
-      <c r="B37" t="s">
-        <v>92</v>
-      </c>
       <c r="C37" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1">
       <c r="A38" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B38" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C38" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B39" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C39" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1">
       <c r="A40" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B40" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="A41" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B41" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3463,7 +3463,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -3493,38 +3493,38 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
@@ -4552,7 +4552,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -4582,24 +4582,24 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -5625,13 +5625,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -5661,12 +5661,12 @@
     </row>
     <row r="2" spans="1:27" ht="14.25" customHeight="1">
       <c r="D2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="14.25" customHeight="1">
       <c r="D3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1"/>

</xml_diff>